<commit_message>
- extracted data from  `10.3390/ma15238546 `
</commit_message>
<xml_diff>
--- a/HighThroughput_Nov2024.xlsx
+++ b/HighThroughput_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DC74C8-EF75-4D4A-8569-BA6E19BDA619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243350A5-124C-5A42-A76E-718C38CAFA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="760" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2360" yWindow="3440" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
   <si>
     <t>Metadata</t>
   </si>
@@ -314,6 +314,78 @@
   <si>
     <t>Col5</t>
   </si>
+  <si>
+    <t>Zr12 Mo23 Ta25 W40</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>Zr19 Mo41 Ta20 W20</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>Zr11 Mo11 Ta25 W53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F6C </t>
+  </si>
+  <si>
+    <t>Zr21 Mo25 Ta25 W29</t>
+  </si>
+  <si>
+    <t>Zr18 Mo18 Ta36 W28</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>Zr29 Mo27 Ta26 W18</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>nanohardness</t>
+  </si>
+  <si>
+    <t>I5 sample ID; magnetron sputtering deposition with Ar at 0.4Pa; 10nm grain size</t>
+  </si>
+  <si>
+    <t>D11 sample ID; magnetron sputtering deposition with Ar at 0.4Pa; 10nm grain size</t>
+  </si>
+  <si>
+    <t>E8 sample ID; magnetron sputtering deposition with Ar at 0.4Pa; 10nm grain size</t>
+  </si>
+  <si>
+    <t>F6C sample ID; magnetron sputtering deposition with Ar at 0.4Pa; 10nm grain size</t>
+  </si>
+  <si>
+    <t>C5 sample ID; magnetron sputtering deposition with Ar at 0.4Pa; 10nm grain size</t>
+  </si>
+  <si>
+    <t>E4 sample ID; magnetron sputtering deposition with Ar at 0.4Pa; 10nm grain size</t>
+  </si>
+  <si>
+    <t>reduced elastic modulus</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.3390/ma15238546 </t>
+  </si>
 </sst>
 </file>
 
@@ -322,7 +394,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +479,18 @@
       <name val="Calibri (Body)"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -917,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1070,6 +1154,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1121,72 +1271,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1494,8 +1579,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1544,19 +1629,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="77"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="60"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1567,17 +1652,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="81"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="64"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1606,43 +1691,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="84" t="s">
+      <c r="E5" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="84" t="s">
+      <c r="F5" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="84" t="s">
+      <c r="G5" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="85" t="s">
+      <c r="H5" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="87" t="s">
+      <c r="I5" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="89" t="s">
+      <c r="J5" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="89" t="s">
+      <c r="K5" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="84" t="s">
+      <c r="L5" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="84" t="s">
+      <c r="M5" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="84" t="s">
+      <c r="N5" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="52" t="s">
+      <c r="O5" s="74" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1653,19 +1738,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="53"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="75"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -1710,7 +1795,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="54"/>
+      <c r="O7" s="76"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -1723,37 +1808,37 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="58" t="s">
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="63" t="s">
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="64"/>
+      <c r="N8" s="86"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="65" t="s">
+      <c r="P8" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="67"/>
-      <c r="T8" s="68"/>
-    </row>
-    <row r="9" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q8" s="88"/>
+      <c r="R8" s="89"/>
+      <c r="S8" s="89"/>
+      <c r="T8" s="90"/>
+    </row>
+    <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>44</v>
       </c>
@@ -1814,205 +1899,517 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="A10" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="9"/>
+      <c r="I10" s="43">
+        <v>298</v>
+      </c>
+      <c r="J10" s="4">
+        <v>12250000000</v>
+      </c>
+      <c r="K10" s="4">
+        <v>750000000</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="A11" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="9"/>
+      <c r="I11" s="43">
+        <v>298</v>
+      </c>
+      <c r="J11" s="4">
+        <v>19920000000</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1000000000</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="O11" s="44"/>
     </row>
     <row r="12" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="A12" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="9"/>
+      <c r="I12" s="43">
+        <v>298</v>
+      </c>
+      <c r="J12" s="4">
+        <v>10360000000</v>
+      </c>
+      <c r="K12" s="4">
+        <v>750000000</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="O12" s="45"/>
     </row>
     <row r="13" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="A13" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="9"/>
+      <c r="I13" s="43">
+        <v>298</v>
+      </c>
+      <c r="J13" s="4">
+        <v>10810000000</v>
+      </c>
+      <c r="K13" s="4">
+        <v>1000000000</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="O13" s="44"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="A14" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="9"/>
+      <c r="I14" s="43">
+        <v>298</v>
+      </c>
+      <c r="J14" s="4">
+        <v>8280000000</v>
+      </c>
+      <c r="K14" s="4">
+        <v>500000000</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="A15" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="91" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="9"/>
+      <c r="I15" s="43">
+        <v>298</v>
+      </c>
+      <c r="J15" s="4">
+        <v>7560000000</v>
+      </c>
+      <c r="K15" s="4">
+        <v>750000000</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="A16" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="91" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="9"/>
+      <c r="I16" s="43">
+        <v>298</v>
+      </c>
+      <c r="J16" s="4">
+        <v>267600000000</v>
+      </c>
+      <c r="K16" s="4">
+        <v>15000000000</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="O16" s="44"/>
     </row>
     <row r="17" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="A17" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="9"/>
+      <c r="I17" s="43">
+        <v>298</v>
+      </c>
+      <c r="J17" s="4">
+        <v>302700000000</v>
+      </c>
+      <c r="K17" s="4">
+        <v>25000000000</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="P17" s="46"/>
       <c r="Q17" s="46"/>
     </row>
     <row r="18" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="9"/>
+      <c r="A18" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="43">
+        <v>298</v>
+      </c>
+      <c r="J18" s="4">
+        <v>215000000000</v>
+      </c>
+      <c r="K18" s="4">
+        <v>10000000000</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="19" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="9"/>
+      <c r="A19" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="43">
+        <v>298</v>
+      </c>
+      <c r="J19" s="4">
+        <v>201200000000</v>
+      </c>
+      <c r="K19" s="4">
+        <v>5000000000</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="20" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="9"/>
+      <c r="A20" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="43">
+        <v>298</v>
+      </c>
+      <c r="J20" s="4">
+        <v>182100000000</v>
+      </c>
+      <c r="K20" s="4">
+        <v>5000000000</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="21" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="9"/>
+      <c r="A21" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="43">
+        <v>298</v>
+      </c>
+      <c r="J21" s="4">
+        <v>140200000000</v>
+      </c>
+      <c r="K21" s="4">
+        <v>5000000000</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24"/>
@@ -8216,6 +8613,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -8230,12 +8632,8 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
   </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- extracted data from  `10.1016/j.jallcom.2015.06.097 `
</commit_message>
<xml_diff>
--- a/HighThroughput_Nov2024.xlsx
+++ b/HighThroughput_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243350A5-124C-5A42-A76E-718C38CAFA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7F9587-EEF3-EC4F-98BB-04819D03868F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2360" yWindow="3440" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="107">
   <si>
     <t>Metadata</t>
   </si>
@@ -385,6 +385,66 @@
   </si>
   <si>
     <t xml:space="preserve">10.3390/ma15238546 </t>
+  </si>
+  <si>
+    <t>CoCrCuFeNi</t>
+  </si>
+  <si>
+    <t>(CoCrCuFeNi)19 Nb5</t>
+  </si>
+  <si>
+    <t>(CoCrCuFeNi)18 Nb10</t>
+  </si>
+  <si>
+    <t>(CoCrCuFeNi)17 Nb15</t>
+  </si>
+  <si>
+    <t>(CoCrCuFeNi)15.4 Nb23</t>
+  </si>
+  <si>
+    <t>NB000</t>
+  </si>
+  <si>
+    <t>NB005</t>
+  </si>
+  <si>
+    <t>NB010</t>
+  </si>
+  <si>
+    <t>NB015</t>
+  </si>
+  <si>
+    <t>NB023</t>
+  </si>
+  <si>
+    <t>NB000; deposited by magnetron sputtering coldpressed powder targets; p*d=2.8 Pa cm</t>
+  </si>
+  <si>
+    <t>FCC</t>
+  </si>
+  <si>
+    <t>FCC+amorphous</t>
+  </si>
+  <si>
+    <t>amorphous</t>
+  </si>
+  <si>
+    <t>NB005; deposited by magnetron sputtering coldpressed powder targets; p*d=2.8 Pa cm</t>
+  </si>
+  <si>
+    <t>NB010; deposited by magnetron sputtering coldpressed powder targets; p*d=2.8 Pa cm</t>
+  </si>
+  <si>
+    <t>NB015; deposited by magnetron sputtering coldpressed powder targets; p*d=2.8 Pa cm</t>
+  </si>
+  <si>
+    <t>NB023; deposited by magnetron sputtering coldpressed powder targets; p*d=2.8 Pa cm</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2015.06.097</t>
   </si>
 </sst>
 </file>
@@ -1579,8 +1639,8 @@
   </sheetPr>
   <dimension ref="A1:T430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2412,11 +2472,21 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="9"/>
+      <c r="A22" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>97</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="42"/>
@@ -2424,15 +2494,29 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="9"/>
+      <c r="M22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="9"/>
+      <c r="A23" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>101</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="42"/>
@@ -2440,15 +2524,29 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="9"/>
+      <c r="M23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="24" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="9"/>
+      <c r="A24" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>102</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="42"/>
@@ -2456,15 +2554,29 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="9"/>
+      <c r="M24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="9"/>
+      <c r="A25" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>103</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="42"/>
@@ -2472,15 +2584,29 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="9"/>
+      <c r="M25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="26" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="44"/>
+      <c r="A26" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>104</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="42"/>
@@ -2488,8 +2614,12 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="9"/>
+      <c r="M26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="27" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="24"/>

</xml_diff>

<commit_message>
- small data fix
</commit_message>
<xml_diff>
--- a/HighThroughput_Nov2024.xlsx
+++ b/HighThroughput_Nov2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E255B4B4-A6D4-4D4F-AAD8-A15E17DA59CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504AB41D-A72A-E044-A904-8142070BBCCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="1580" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="142">
   <si>
     <t>Metadata</t>
   </si>
@@ -1744,8 +1744,8 @@
   </sheetPr>
   <dimension ref="A1:T428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2593,7 +2593,9 @@
         <v>97</v>
       </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H22" s="42"/>
       <c r="I22" s="3"/>
       <c r="J22" s="4"/>
@@ -2623,7 +2625,9 @@
         <v>101</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H23" s="42"/>
       <c r="I23" s="3"/>
       <c r="J23" s="4"/>
@@ -2653,7 +2657,9 @@
         <v>102</v>
       </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H24" s="42"/>
       <c r="I24" s="3"/>
       <c r="J24" s="4"/>
@@ -2683,7 +2689,9 @@
         <v>103</v>
       </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H25" s="42"/>
       <c r="I25" s="3"/>
       <c r="J25" s="4"/>
@@ -2713,7 +2721,9 @@
         <v>104</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H26" s="42"/>
       <c r="I26" s="3"/>
       <c r="J26" s="4"/>
@@ -2743,7 +2753,9 @@
       <c r="F27" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H27" s="42" t="s">
         <v>131</v>
       </c>
@@ -2783,7 +2795,9 @@
       <c r="F28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H28" s="42" t="s">
         <v>131</v>
       </c>
@@ -2823,7 +2837,9 @@
       <c r="F29" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H29" s="42" t="s">
         <v>131</v>
       </c>
@@ -2863,7 +2879,9 @@
       <c r="F30" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H30" s="42" t="s">
         <v>131</v>
       </c>
@@ -2903,7 +2921,9 @@
       <c r="F31" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H31" s="42" t="s">
         <v>131</v>
       </c>
@@ -2943,7 +2963,9 @@
       <c r="F32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H32" s="42" t="s">
         <v>131</v>
       </c>
@@ -2983,7 +3005,9 @@
       <c r="F33" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H33" s="42" t="s">
         <v>131</v>
       </c>
@@ -3023,7 +3047,9 @@
       <c r="F34" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H34" s="42" t="s">
         <v>131</v>
       </c>
@@ -3063,7 +3089,9 @@
       <c r="F35" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H35" s="42" t="s">
         <v>131</v>
       </c>
@@ -3103,7 +3131,9 @@
       <c r="F36" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H36" s="42" t="s">
         <v>131</v>
       </c>
@@ -3143,7 +3173,9 @@
       <c r="F37" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H37" s="42" t="s">
         <v>131</v>
       </c>
@@ -3183,7 +3215,9 @@
       <c r="F38" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H38" s="42" t="s">
         <v>131</v>
       </c>
@@ -3223,7 +3257,9 @@
       <c r="F39" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G39" s="42"/>
+      <c r="G39" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H39" s="42" t="s">
         <v>131</v>
       </c>
@@ -3263,7 +3299,9 @@
       <c r="F40" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G40" s="42"/>
+      <c r="G40" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H40" s="42" t="s">
         <v>131</v>
       </c>
@@ -3303,7 +3341,9 @@
       <c r="F41" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G41" s="42"/>
+      <c r="G41" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H41" s="42" t="s">
         <v>131</v>
       </c>
@@ -3343,7 +3383,9 @@
       <c r="F42" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G42" s="42"/>
+      <c r="G42" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H42" s="42" t="s">
         <v>131</v>
       </c>
@@ -3383,7 +3425,9 @@
       <c r="F43" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G43" s="42"/>
+      <c r="G43" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H43" s="42" t="s">
         <v>131</v>
       </c>
@@ -3423,7 +3467,9 @@
       <c r="F44" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G44" s="42"/>
+      <c r="G44" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H44" s="42" t="s">
         <v>131</v>
       </c>
@@ -3463,7 +3509,9 @@
       <c r="F45" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G45" s="42"/>
+      <c r="G45" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H45" s="42" t="s">
         <v>131</v>
       </c>
@@ -3503,7 +3551,9 @@
       <c r="F46" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G46" s="42"/>
+      <c r="G46" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H46" s="42" t="s">
         <v>131</v>
       </c>
@@ -3543,7 +3593,9 @@
       <c r="F47" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G47" s="42"/>
+      <c r="G47" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H47" s="42" t="s">
         <v>131</v>
       </c>
@@ -3583,7 +3635,9 @@
       <c r="F48" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G48" s="42"/>
+      <c r="G48" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H48" s="42" t="s">
         <v>131</v>
       </c>
@@ -3623,7 +3677,9 @@
       <c r="F49" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G49" s="42"/>
+      <c r="G49" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H49" s="42" t="s">
         <v>131</v>
       </c>
@@ -3663,7 +3719,9 @@
       <c r="F50" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G50" s="42"/>
+      <c r="G50" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H50" s="42" t="s">
         <v>131</v>
       </c>
@@ -3705,7 +3763,9 @@
       <c r="F51" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G51" s="42"/>
+      <c r="G51" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H51" s="42" t="s">
         <v>131</v>
       </c>
@@ -3747,7 +3807,9 @@
       <c r="F52" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G52" s="42"/>
+      <c r="G52" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H52" s="42" t="s">
         <v>131</v>
       </c>
@@ -3789,7 +3851,9 @@
       <c r="F53" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G53" s="42"/>
+      <c r="G53" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H53" s="42" t="s">
         <v>131</v>
       </c>
@@ -3831,7 +3895,9 @@
       <c r="F54" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G54" s="42"/>
+      <c r="G54" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H54" s="42" t="s">
         <v>131</v>
       </c>
@@ -3873,7 +3939,9 @@
       <c r="F55" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G55" s="42"/>
+      <c r="G55" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H55" s="42" t="s">
         <v>131</v>
       </c>
@@ -3915,7 +3983,9 @@
       <c r="F56" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G56" s="42"/>
+      <c r="G56" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H56" s="42" t="s">
         <v>131</v>
       </c>
@@ -3957,7 +4027,9 @@
       <c r="F57" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G57" s="42"/>
+      <c r="G57" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H57" s="42" t="s">
         <v>131</v>
       </c>
@@ -3999,7 +4071,9 @@
       <c r="F58" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G58" s="42"/>
+      <c r="G58" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H58" s="42" t="s">
         <v>131</v>
       </c>
@@ -4039,7 +4113,9 @@
       <c r="F59" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G59" s="42"/>
+      <c r="G59" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H59" s="42" t="s">
         <v>131</v>
       </c>
@@ -4079,7 +4155,9 @@
       <c r="F60" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G60" s="42"/>
+      <c r="G60" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H60" s="42" t="s">
         <v>131</v>
       </c>
@@ -4119,7 +4197,9 @@
       <c r="F61" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G61" s="42"/>
+      <c r="G61" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H61" s="42" t="s">
         <v>131</v>
       </c>
@@ -4159,7 +4239,9 @@
       <c r="F62" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G62" s="42"/>
+      <c r="G62" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H62" s="42" t="s">
         <v>131</v>
       </c>
@@ -4199,7 +4281,9 @@
       <c r="F63" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G63" s="42"/>
+      <c r="G63" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H63" s="42" t="s">
         <v>131</v>
       </c>
@@ -4239,7 +4323,9 @@
       <c r="F64" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G64" s="42"/>
+      <c r="G64" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H64" s="42" t="s">
         <v>131</v>
       </c>
@@ -4279,7 +4365,9 @@
       <c r="F65" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G65" s="42"/>
+      <c r="G65" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H65" s="42" t="s">
         <v>131</v>
       </c>
@@ -4319,7 +4407,9 @@
       <c r="F66" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G66" s="42"/>
+      <c r="G66" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H66" s="42" t="s">
         <v>131</v>
       </c>
@@ -4359,7 +4449,9 @@
       <c r="F67" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G67" s="42"/>
+      <c r="G67" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H67" s="42" t="s">
         <v>131</v>
       </c>
@@ -4399,7 +4491,9 @@
       <c r="F68" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G68" s="42"/>
+      <c r="G68" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H68" s="42" t="s">
         <v>131</v>
       </c>
@@ -4439,7 +4533,9 @@
       <c r="F69" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G69" s="42"/>
+      <c r="G69" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H69" s="42" t="s">
         <v>131</v>
       </c>
@@ -4479,7 +4575,9 @@
       <c r="F70" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G70" s="42"/>
+      <c r="G70" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H70" s="42" t="s">
         <v>131</v>
       </c>
@@ -4519,7 +4617,9 @@
       <c r="F71" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G71" s="42"/>
+      <c r="G71" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H71" s="42" t="s">
         <v>131</v>
       </c>
@@ -4559,7 +4659,9 @@
       <c r="F72" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G72" s="42"/>
+      <c r="G72" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H72" s="42" t="s">
         <v>131</v>
       </c>
@@ -4599,7 +4701,9 @@
       <c r="F73" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G73" s="42"/>
+      <c r="G73" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H73" s="42" t="s">
         <v>131</v>
       </c>
@@ -4639,7 +4743,9 @@
       <c r="F74" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G74" s="42"/>
+      <c r="G74" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H74" s="42" t="s">
         <v>131</v>
       </c>
@@ -4679,7 +4785,9 @@
       <c r="F75" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G75" s="42"/>
+      <c r="G75" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H75" s="42" t="s">
         <v>131</v>
       </c>
@@ -4719,7 +4827,9 @@
       <c r="F76" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="42"/>
+      <c r="G76" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H76" s="42" t="s">
         <v>131</v>
       </c>
@@ -4759,7 +4869,9 @@
       <c r="F77" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G77" s="42"/>
+      <c r="G77" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H77" s="42" t="s">
         <v>131</v>
       </c>
@@ -4799,7 +4911,9 @@
       <c r="F78" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G78" s="42"/>
+      <c r="G78" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H78" s="42" t="s">
         <v>131</v>
       </c>
@@ -4839,7 +4953,9 @@
       <c r="F79" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G79" s="42"/>
+      <c r="G79" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H79" s="42" t="s">
         <v>131</v>
       </c>
@@ -4879,7 +4995,9 @@
       <c r="F80" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G80" s="42"/>
+      <c r="G80" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H80" s="42" t="s">
         <v>131</v>
       </c>
@@ -4917,7 +5035,9 @@
       <c r="F81" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G81" s="42"/>
+      <c r="G81" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H81" s="42" t="s">
         <v>131</v>
       </c>
@@ -4957,7 +5077,9 @@
       <c r="F82" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G82" s="42"/>
+      <c r="G82" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H82" s="42" t="s">
         <v>131</v>
       </c>
@@ -4997,7 +5119,9 @@
       <c r="F83" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G83" s="42"/>
+      <c r="G83" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H83" s="42" t="s">
         <v>131</v>
       </c>
@@ -5037,7 +5161,9 @@
       <c r="F84" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G84" s="42"/>
+      <c r="G84" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H84" s="42" t="s">
         <v>131</v>
       </c>
@@ -5077,7 +5203,9 @@
       <c r="F85" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G85" s="42"/>
+      <c r="G85" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H85" s="42" t="s">
         <v>131</v>
       </c>
@@ -5117,7 +5245,9 @@
       <c r="F86" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G86" s="42"/>
+      <c r="G86" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H86" s="42" t="s">
         <v>131</v>
       </c>
@@ -5157,7 +5287,9 @@
       <c r="F87" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G87" s="42"/>
+      <c r="G87" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H87" s="42" t="s">
         <v>131</v>
       </c>
@@ -5197,7 +5329,9 @@
       <c r="F88" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G88" s="42"/>
+      <c r="G88" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H88" s="42" t="s">
         <v>131</v>
       </c>
@@ -5237,7 +5371,9 @@
       <c r="F89" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G89" s="42"/>
+      <c r="G89" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H89" s="42" t="s">
         <v>131</v>
       </c>
@@ -5277,7 +5413,9 @@
       <c r="F90" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="G90" s="42"/>
+      <c r="G90" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H90" s="42" t="s">
         <v>131</v>
       </c>
@@ -5317,7 +5455,9 @@
       <c r="F91" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G91" s="42"/>
+      <c r="G91" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H91" s="42" t="s">
         <v>131</v>
       </c>
@@ -5355,7 +5495,9 @@
       <c r="F92" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G92" s="42"/>
+      <c r="G92" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H92" s="42" t="s">
         <v>131</v>
       </c>
@@ -5393,7 +5535,9 @@
       <c r="F93" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G93" s="42"/>
+      <c r="G93" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H93" s="42" t="s">
         <v>131</v>
       </c>
@@ -5431,7 +5575,9 @@
       <c r="F94" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G94" s="42"/>
+      <c r="G94" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H94" s="42" t="s">
         <v>131</v>
       </c>
@@ -5469,7 +5615,9 @@
       <c r="F95" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G95" s="42"/>
+      <c r="G95" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H95" s="42" t="s">
         <v>131</v>
       </c>
@@ -5507,7 +5655,9 @@
       <c r="F96" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G96" s="42"/>
+      <c r="G96" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H96" s="42" t="s">
         <v>131</v>
       </c>
@@ -5545,7 +5695,9 @@
       <c r="F97" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G97" s="42"/>
+      <c r="G97" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H97" s="42" t="s">
         <v>131</v>
       </c>
@@ -5583,7 +5735,9 @@
       <c r="F98" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G98" s="42"/>
+      <c r="G98" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H98" s="42" t="s">
         <v>131</v>
       </c>
@@ -5621,7 +5775,9 @@
       <c r="F99" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G99" s="42"/>
+      <c r="G99" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H99" s="42" t="s">
         <v>131</v>
       </c>
@@ -5659,7 +5815,9 @@
       <c r="F100" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="G100" s="42"/>
+      <c r="G100" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H100" s="42" t="s">
         <v>131</v>
       </c>
@@ -5697,7 +5855,9 @@
       <c r="F101" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G101" s="42"/>
+      <c r="G101" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H101" s="42" t="s">
         <v>131</v>
       </c>
@@ -5735,7 +5895,9 @@
       <c r="F102" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G102" s="42"/>
+      <c r="G102" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H102" s="42" t="s">
         <v>131</v>
       </c>
@@ -5773,7 +5935,9 @@
       <c r="F103" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G103" s="42"/>
+      <c r="G103" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H103" s="42" t="s">
         <v>131</v>
       </c>
@@ -5811,7 +5975,9 @@
       <c r="F104" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G104" s="42"/>
+      <c r="G104" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H104" s="42" t="s">
         <v>131</v>
       </c>
@@ -5849,7 +6015,9 @@
       <c r="F105" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G105" s="42"/>
+      <c r="G105" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H105" s="42" t="s">
         <v>131</v>
       </c>
@@ -5887,7 +6055,9 @@
       <c r="F106" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="G106" s="42"/>
+      <c r="G106" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H106" s="42" t="s">
         <v>131</v>
       </c>
@@ -5925,7 +6095,9 @@
       <c r="F107" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="G107" s="42"/>
+      <c r="G107" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H107" s="42" t="s">
         <v>131</v>
       </c>
@@ -5963,7 +6135,9 @@
       <c r="F108" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="G108" s="42"/>
+      <c r="G108" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H108" s="42" t="s">
         <v>131</v>
       </c>
@@ -6001,7 +6175,9 @@
       <c r="F109" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="G109" s="42"/>
+      <c r="G109" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H109" s="42" t="s">
         <v>131</v>
       </c>
@@ -6039,7 +6215,9 @@
       <c r="F110" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="G110" s="42"/>
+      <c r="G110" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H110" s="42" t="s">
         <v>131</v>
       </c>
@@ -6077,7 +6255,9 @@
       <c r="F111" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="G111" s="42"/>
+      <c r="G111" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H111" s="42" t="s">
         <v>131</v>
       </c>
@@ -6115,7 +6295,9 @@
       <c r="F112" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="G112" s="42"/>
+      <c r="G112" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H112" s="42" t="s">
         <v>131</v>
       </c>
@@ -6153,7 +6335,9 @@
       <c r="F113" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="G113" s="42"/>
+      <c r="G113" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H113" s="42" t="s">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
- extracted HT data from `10.1088/2631-7990/abcca8`
</commit_message>
<xml_diff>
--- a/HighThroughput_Nov2024.xlsx
+++ b/HighThroughput_Nov2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD6CF7-CEF3-2547-BA95-26E8C2CA5128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DC2B77-D69B-984D-9CB9-9B58476CF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="1580" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9220" yWindow="2600" windowWidth="31640" windowHeight="18260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6723" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6931" uniqueCount="473">
   <si>
     <t>Metadata</t>
   </si>
@@ -1492,6 +1492,57 @@
   </si>
   <si>
     <t>10.1007/s44210-022-00007-3</t>
+  </si>
+  <si>
+    <t>Ti22Zr22Nb42Hf7Ta7</t>
+  </si>
+  <si>
+    <t>Ti22Zr42Nb22Hf7Ta7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti42Zr22Nb22Hf7Ta7 </t>
+  </si>
+  <si>
+    <t>Ti27Zr27Nb27Hf9.5Ta9.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti33.3Zr33.3Nb33.3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zr33.3Nb33.3Ta33.3 </t>
+  </si>
+  <si>
+    <t>Ti25Zr25Nb25Ta25</t>
+  </si>
+  <si>
+    <t>TiZrNbHfTa</t>
+  </si>
+  <si>
+    <t>SLM</t>
+  </si>
+  <si>
+    <t>(TiZrNbHfTa)19.46 O1.9 N0.8</t>
+  </si>
+  <si>
+    <t>LMD of elemental powder blends on a 3 mm-thick Ti substrate in Ar; built vertically into columns; high-interstitial contamination feedstock</t>
+  </si>
+  <si>
+    <t>LMD of elemental powder blends on a 3 mm-thick Ti substrate in Ar; built vertically into columns; higher purity feedstock</t>
+  </si>
+  <si>
+    <t>hardness</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>strain rate of 1e−3/s</t>
+  </si>
+  <si>
+    <t>10.1088/2631-7990/abcca8</t>
   </si>
 </sst>
 </file>
@@ -2262,6 +2313,57 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2327,57 +2429,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2684,10 +2735,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T735"/>
+  <dimension ref="A1:T759"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="94" workbookViewId="0">
-      <selection activeCell="H739" sqref="H739"/>
+    <sheetView tabSelected="1" topLeftCell="J723" zoomScale="94" workbookViewId="0">
+      <selection activeCell="O759" sqref="O759"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2736,19 +2787,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="61"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="78"/>
       <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2759,17 +2810,17 @@
         <v>5</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="65"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2798,43 +2849,43 @@
       <c r="B5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="D5" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="68" t="s">
+      <c r="L5" s="85" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="68" t="s">
+      <c r="N5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="75" t="s">
+      <c r="O5" s="53" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2845,19 +2896,19 @@
       <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="76"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="84"/>
+      <c r="N6" s="84"/>
+      <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:20" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
@@ -2902,7 +2953,7 @@
       <c r="N7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="77"/>
+      <c r="O7" s="55"/>
       <c r="P7" s="21" t="s">
         <v>36</v>
       </c>
@@ -2915,35 +2966,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="81" t="s">
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="86" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="N8" s="87"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="88" t="s">
+      <c r="P8" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="91"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="69"/>
     </row>
     <row r="9" spans="1:20" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
@@ -33424,13 +33475,958 @@
         <v>165.8</v>
       </c>
     </row>
+    <row r="736" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B736" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="C736" s="42"/>
+      <c r="D736" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E736" s="44" t="s">
+        <v>466</v>
+      </c>
+      <c r="F736" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="G736" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H736" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I736" s="3">
+        <v>298</v>
+      </c>
+      <c r="J736" s="50">
+        <v>1900000000</v>
+      </c>
+      <c r="L736" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M736" s="51" t="s">
+        <v>470</v>
+      </c>
+      <c r="N736" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="737" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B737" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="C737" s="42"/>
+      <c r="D737" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E737" s="44" t="s">
+        <v>466</v>
+      </c>
+      <c r="F737" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="G737" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H737" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I737" s="3">
+        <v>298</v>
+      </c>
+      <c r="J737" s="50">
+        <v>22</v>
+      </c>
+      <c r="L737" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="M737" s="51" t="s">
+        <v>470</v>
+      </c>
+      <c r="N737" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="738" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B738" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="C738" s="42"/>
+      <c r="D738" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E738" s="44" t="s">
+        <v>466</v>
+      </c>
+      <c r="F738" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G738" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H738" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I738" s="3">
+        <v>298</v>
+      </c>
+      <c r="J738" s="50">
+        <v>1460000000</v>
+      </c>
+      <c r="K738" s="50">
+        <v>30000000</v>
+      </c>
+      <c r="L738" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M738" s="51" t="s">
+        <v>470</v>
+      </c>
+      <c r="N738" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="739" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B739" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="C739" s="42"/>
+      <c r="D739" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E739" s="44" t="s">
+        <v>466</v>
+      </c>
+      <c r="F739" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G739" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H739" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I739" s="3">
+        <v>298</v>
+      </c>
+      <c r="J739" s="50">
+        <f>P739*9807000</f>
+        <v>4471992000</v>
+      </c>
+      <c r="K739" s="50">
+        <f>Q739*9807000</f>
+        <v>147105000</v>
+      </c>
+      <c r="L739" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M739" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N739" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P739" s="6">
+        <v>456</v>
+      </c>
+      <c r="Q739" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="740" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B740" s="44" t="s">
+        <v>463</v>
+      </c>
+      <c r="C740" s="42"/>
+      <c r="D740" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E740" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F740" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G740" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H740" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I740" s="3">
+        <v>298</v>
+      </c>
+      <c r="J740" s="50">
+        <f t="shared" ref="J740:J747" si="10">P740*9807000</f>
+        <v>3373608000</v>
+      </c>
+      <c r="K740" s="50">
+        <f t="shared" ref="K740:K747" si="11">Q740*9807000</f>
+        <v>147105000</v>
+      </c>
+      <c r="L740" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M740" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N740" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P740" s="6">
+        <v>344</v>
+      </c>
+      <c r="Q740" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="741" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B741" s="44" t="s">
+        <v>462</v>
+      </c>
+      <c r="C741" s="42"/>
+      <c r="D741" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E741" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F741" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G741" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H741" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I741" s="3">
+        <v>298</v>
+      </c>
+      <c r="J741" s="50">
+        <f t="shared" si="10"/>
+        <v>3491292000</v>
+      </c>
+      <c r="K741" s="50">
+        <f t="shared" si="11"/>
+        <v>147105000</v>
+      </c>
+      <c r="L741" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M741" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N741" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P741" s="6">
+        <v>356</v>
+      </c>
+      <c r="Q741" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="742" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B742" s="44" t="s">
+        <v>461</v>
+      </c>
+      <c r="C742" s="42"/>
+      <c r="D742" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E742" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F742" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G742" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H742" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I742" s="3">
+        <v>298</v>
+      </c>
+      <c r="J742" s="50">
+        <f t="shared" si="10"/>
+        <v>3608976000</v>
+      </c>
+      <c r="K742" s="50">
+        <f t="shared" si="11"/>
+        <v>147105000</v>
+      </c>
+      <c r="L742" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M742" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N742" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P742" s="6">
+        <v>368</v>
+      </c>
+      <c r="Q742" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="743" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B743" s="44" t="s">
+        <v>460</v>
+      </c>
+      <c r="C743" s="42"/>
+      <c r="D743" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E743" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F743" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G743" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H743" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I743" s="3">
+        <v>298</v>
+      </c>
+      <c r="J743" s="50">
+        <f t="shared" si="10"/>
+        <v>2834223000</v>
+      </c>
+      <c r="K743" s="50">
+        <f t="shared" si="11"/>
+        <v>147105000</v>
+      </c>
+      <c r="L743" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M743" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N743" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P743" s="6">
+        <v>289</v>
+      </c>
+      <c r="Q743" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="744" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B744" s="44" t="s">
+        <v>459</v>
+      </c>
+      <c r="C744" s="42"/>
+      <c r="D744" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E744" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F744" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G744" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H744" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I744" s="3">
+        <v>298</v>
+      </c>
+      <c r="J744" s="50">
+        <f t="shared" si="10"/>
+        <v>3187275000</v>
+      </c>
+      <c r="K744" s="50">
+        <f t="shared" si="11"/>
+        <v>147105000</v>
+      </c>
+      <c r="L744" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M744" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N744" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P744" s="6">
+        <v>325</v>
+      </c>
+      <c r="Q744" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="745" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B745" s="44" t="s">
+        <v>458</v>
+      </c>
+      <c r="C745" s="42"/>
+      <c r="D745" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E745" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F745" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G745" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H745" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I745" s="3">
+        <v>298</v>
+      </c>
+      <c r="J745" s="50">
+        <f t="shared" si="10"/>
+        <v>2696925000</v>
+      </c>
+      <c r="K745" s="50">
+        <f t="shared" si="11"/>
+        <v>147105000</v>
+      </c>
+      <c r="L745" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M745" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N745" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P745" s="6">
+        <v>275</v>
+      </c>
+      <c r="Q745" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="746" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B746" s="44" t="s">
+        <v>457</v>
+      </c>
+      <c r="D746" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E746" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F746" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G746" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H746" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I746" s="3">
+        <v>298</v>
+      </c>
+      <c r="J746" s="50">
+        <f t="shared" si="10"/>
+        <v>2863644000</v>
+      </c>
+      <c r="K746" s="50">
+        <f t="shared" si="11"/>
+        <v>147105000</v>
+      </c>
+      <c r="L746" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M746" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N746" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P746" s="6">
+        <v>292</v>
+      </c>
+      <c r="Q746" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="747" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B747" s="44" t="s">
+        <v>456</v>
+      </c>
+      <c r="D747" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E747" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F747" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="G747" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H747" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I747" s="3">
+        <v>298</v>
+      </c>
+      <c r="J747" s="50">
+        <f t="shared" si="10"/>
+        <v>2863644000</v>
+      </c>
+      <c r="K747" s="50">
+        <f t="shared" si="11"/>
+        <v>147105000</v>
+      </c>
+      <c r="L747" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M747" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N747" s="51" t="s">
+        <v>472</v>
+      </c>
+      <c r="P747" s="6">
+        <v>292</v>
+      </c>
+      <c r="Q747" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="748" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B748" s="44" t="s">
+        <v>463</v>
+      </c>
+      <c r="C748" s="42"/>
+      <c r="D748" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E748" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F748" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G748" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H748" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I748" s="3">
+        <v>298</v>
+      </c>
+      <c r="J748" s="50">
+        <v>1105000000</v>
+      </c>
+      <c r="K748" s="50">
+        <v>10000000</v>
+      </c>
+      <c r="L748" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M748" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N748" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="749" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B749" s="44" t="s">
+        <v>460</v>
+      </c>
+      <c r="C749" s="42"/>
+      <c r="D749" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E749" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F749" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G749" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H749" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I749" s="3">
+        <v>298</v>
+      </c>
+      <c r="J749" s="50">
+        <v>795000000</v>
+      </c>
+      <c r="K749" s="50">
+        <v>4000000</v>
+      </c>
+      <c r="L749" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M749" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N749" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="750" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B750" s="44" t="s">
+        <v>459</v>
+      </c>
+      <c r="C750" s="42"/>
+      <c r="D750" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E750" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F750" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G750" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H750" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I750" s="3">
+        <v>298</v>
+      </c>
+      <c r="J750" s="50">
+        <v>910000000</v>
+      </c>
+      <c r="K750" s="50">
+        <v>50000000</v>
+      </c>
+      <c r="L750" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M750" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N750" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="751" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B751" s="44" t="s">
+        <v>458</v>
+      </c>
+      <c r="C751" s="42"/>
+      <c r="D751" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E751" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F751" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G751" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H751" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I751" s="3">
+        <v>298</v>
+      </c>
+      <c r="J751" s="50">
+        <v>840000000</v>
+      </c>
+      <c r="K751" s="50">
+        <v>30000000</v>
+      </c>
+      <c r="L751" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M751" s="51" t="s">
+        <v>469</v>
+      </c>
+      <c r="N751" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="752" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B752" s="44" t="s">
+        <v>463</v>
+      </c>
+      <c r="C752" s="42"/>
+      <c r="D752" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E752" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F752" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G752" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H752" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I752" s="3">
+        <v>298</v>
+      </c>
+      <c r="J752" s="50">
+        <v>40</v>
+      </c>
+      <c r="L752" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="N752" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="753" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B753" s="44" t="s">
+        <v>462</v>
+      </c>
+      <c r="C753" s="42"/>
+      <c r="D753" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E753" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F753" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G753" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H753" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I753" s="3">
+        <v>298</v>
+      </c>
+      <c r="J753" s="50">
+        <v>40</v>
+      </c>
+      <c r="L753" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="N753" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="754" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B754" s="44" t="s">
+        <v>461</v>
+      </c>
+      <c r="C754" s="42"/>
+      <c r="D754" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E754" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F754" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G754" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H754" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I754" s="3">
+        <v>298</v>
+      </c>
+      <c r="J754" s="50">
+        <v>40</v>
+      </c>
+      <c r="L754" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="N754" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="755" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B755" s="44" t="s">
+        <v>460</v>
+      </c>
+      <c r="C755" s="42"/>
+      <c r="D755" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E755" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F755" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G755" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H755" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I755" s="3">
+        <v>298</v>
+      </c>
+      <c r="J755" s="50">
+        <v>40</v>
+      </c>
+      <c r="L755" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="N755" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="756" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B756" s="44" t="s">
+        <v>459</v>
+      </c>
+      <c r="C756" s="42"/>
+      <c r="D756" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E756" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F756" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G756" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H756" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I756" s="3">
+        <v>298</v>
+      </c>
+      <c r="J756" s="50">
+        <v>40</v>
+      </c>
+      <c r="L756" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="N756" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="757" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B757" s="44" t="s">
+        <v>458</v>
+      </c>
+      <c r="C757" s="42"/>
+      <c r="D757" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E757" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F757" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G757" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H757" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I757" s="3">
+        <v>298</v>
+      </c>
+      <c r="J757" s="50">
+        <v>40</v>
+      </c>
+      <c r="L757" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="N757" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="758" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B758" s="44" t="s">
+        <v>457</v>
+      </c>
+      <c r="D758" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E758" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F758" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G758" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H758" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I758" s="3">
+        <v>298</v>
+      </c>
+      <c r="J758" s="50">
+        <v>40</v>
+      </c>
+      <c r="L758" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="N758" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="759" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B759" s="44" t="s">
+        <v>456</v>
+      </c>
+      <c r="D759" s="42" t="s">
+        <v>464</v>
+      </c>
+      <c r="E759" s="44" t="s">
+        <v>467</v>
+      </c>
+      <c r="F759" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G759" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="H759" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I759" s="3">
+        <v>298</v>
+      </c>
+      <c r="J759" s="50">
+        <v>40</v>
+      </c>
+      <c r="L759" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="N759" s="51" t="s">
+        <v>472</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="P8:T8"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="C5:C6"/>
@@ -33445,6 +34441,11 @@
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="P8:T8"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>